<commit_message>
UPDATE: feature change and Model change
</commit_message>
<xml_diff>
--- a/Data/predictions.xlsx
+++ b/Data/predictions.xlsx
@@ -802,7 +802,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -914,7 +914,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -1082,7 +1082,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -1194,7 +1194,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -1634,7 +1634,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151">
@@ -3402,7 +3402,7 @@
         <v>370</v>
       </c>
       <c r="B371" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="372">
@@ -3690,7 +3690,7 @@
         <v>406</v>
       </c>
       <c r="B407" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="408">
@@ -3746,7 +3746,7 @@
         <v>413</v>
       </c>
       <c r="B414" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="415">
@@ -4930,7 +4930,7 @@
         <v>561</v>
       </c>
       <c r="B562" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="563">

</xml_diff>